<commit_message>
Work on docs | Updated privacy policy
</commit_message>
<xml_diff>
--- a/public/static/console/templates/coa_templates/standard_coa_template.xlsx
+++ b/public/static/console/templates/coa_templates/standard_coa_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keega\Documents\cannlytics\cannlytics\console\static\console\templates\coa_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A299A53-1F79-4C0E-8ECB-50DC45364628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E636084-8753-446D-8850-2658E104717E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11760" xr2:uid="{3DC962A0-F07A-4786-BEA5-B53141FC009B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +31,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Analyte</t>
+  </si>
+  <si>
+    <t>CBD</t>
+  </si>
+  <si>
+    <t>{{ cbd }}</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,12 +397,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F227385D-FE91-4270-A1ED-7100C5773322}">
-  <dimension ref="A1"/>
+  <dimension ref="B5:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>